<commit_message>
dynamic category and image
</commit_message>
<xml_diff>
--- a/media/quiz/IOM_2019.xlsx
+++ b/media/quiz/IOM_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ExcelConvertable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PYQ-ExcelAndMedias\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F3E159-A061-42A4-B3E6-1547DA420CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0631D09B-FF79-465D-A6FB-F541402EBE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="1215" windowWidth="15375" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="486">
   <si>
     <t>Question</t>
   </si>
@@ -1472,6 +1472,12 @@
   </si>
   <si>
     <t>MAT</t>
+  </si>
+  <si>
+    <t>QuestionImages</t>
+  </si>
+  <si>
+    <t>images/qn1_image.jpeg,images/qn2_image.jpg</t>
   </si>
 </sst>
 </file>
@@ -1848,23 +1854,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D70" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="P73" sqref="P73"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="151" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1886,8 +1894,11 @@
       <c r="G1" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1909,8 +1920,11 @@
       <c r="G2" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1930,7 +1944,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1953,7 +1967,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1976,7 +1990,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1999,7 +2013,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2022,7 +2036,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2045,7 +2059,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2068,7 +2082,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2091,7 +2105,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2114,7 +2128,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2137,7 +2151,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2160,7 +2174,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2183,7 +2197,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -2206,7 +2220,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>

</xml_diff>